<commit_message>
IMDb data collection project
</commit_message>
<xml_diff>
--- a/5LD_DarbasSuTinklalapiais/Filmai.xlsx
+++ b/5LD_DarbasSuTinklalapiais/Filmai.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vult-my.sharepoint.com/personal/laura_ringiene_mif_vu_lt/Documents/paskaitos/RPA/2025/Filmu_Informacija (1)/Filmu_Informacija/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nojus\Documents\UiPath\5LD_DarbasSuTinklalapiais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{D9DD5B52-974B-45B8-A7C6-63CF372D2B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{846AD42C-B29A-44E3-99FB-E2C6F3C5C83A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB3D073-719F-45C4-9828-481C81C5F5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{42BDB03F-5F77-4F35-9FE4-C532E789F044}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42BDB03F-5F77-4F35-9FE4-C532E789F044}"/>
   </bookViews>
   <sheets>
     <sheet name="Filmai" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Filmo pavadinimas</t>
   </si>
@@ -57,19 +57,91 @@
     <t>Ledynmetis</t>
   </si>
   <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>7.5</t>
+  </si>
+  <si>
+    <t>1,447</t>
+  </si>
+  <si>
+    <t>Didėjo</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
     <t>Zootropolis</t>
   </si>
   <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>8.0</t>
+  </si>
+  <si>
+    <t>612</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
     <t>Išvirkščias pasaulis</t>
   </si>
   <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>1,077</t>
+  </si>
+  <si>
+    <t>Mažėjo</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
     <t>Aukštyn</t>
   </si>
   <si>
+    <t>2009</t>
+  </si>
+  <si>
+    <t>8.3</t>
+  </si>
+  <si>
+    <t>1,022</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
     <t>La troškinys</t>
   </si>
   <si>
+    <t>2007</t>
+  </si>
+  <si>
+    <t>537</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
     <t>Vajana</t>
+  </si>
+  <si>
+    <t>7.6</t>
+  </si>
+  <si>
+    <t>486</t>
+  </si>
+  <si>
+    <t>133</t>
   </si>
 </sst>
 </file>
@@ -120,9 +192,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Įprastas" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="186"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -135,8 +227,23 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14BEE08D-B45F-4AD9-8514-98150D2D7CF1}" name="Lentelė1" displayName="Lentelė1" ref="A1:F7" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:F7" xr:uid="{14BEE08D-B45F-4AD9-8514-98150D2D7CF1}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{7DCCC111-8B52-4F14-B9E3-7E00A48B2B64}" name="Filmo pavadinimas"/>
+    <tableColumn id="2" xr3:uid="{DFABB91C-52B2-45A8-985A-5FD7608E8E6B}" name="Išleidimo metai"/>
+    <tableColumn id="3" xr3:uid="{9B656E42-9373-4376-A420-DA271DB0B14E}" name="IMDb reitingas"/>
+    <tableColumn id="4" xr3:uid="{13F6648A-C71C-4F7A-82F5-E59E4D0FFCF2}" name="Populiarumo vieta"/>
+    <tableColumn id="5" xr3:uid="{D859C430-16D5-45C6-9D2F-2C93054E3DF1}" name="Populiarumas didėjo/mažėjo"/>
+    <tableColumn id="6" xr3:uid="{CEF670BE-0A2F-425B-B4F6-2CACFBC25B64}" name="Didėjimo/mažėjimo vietų skaičius"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="„Office“ tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -441,11 +548,11 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -472,34 +579,127 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
         <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>